<commit_message>
Fixed get hosts inventory and more multiple concurrent file deletion
</commit_message>
<xml_diff>
--- a/easyops/static/server_templates/servers_example.xlsx
+++ b/easyops/static/server_templates/servers_example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F96771-1BA2-B241-A5E7-98DE899B586A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57E35D9-5832-104B-AC2B-9BEF009D54DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,52 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>root</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OpenStack_Controller01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OpenStack_Compute01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OpenStack_Compute02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.10.201</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.10.202</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.10.203</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CarltonXu_DEV</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.10.68</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HyperMotion</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>192.168.10.106</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>IP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -89,19 +49,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OpenStack_Controller</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OpenStack_Compute</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dev</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Migration</t>
+    <t>Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.10.33</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -133,27 +89,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -162,11 +103,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,136 +450,89 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>18</v>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>22</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="2">
-        <v>22</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>20</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>